<commit_message>
backup kut files commit hopelijk niks kapot
</commit_message>
<xml_diff>
--- a/Documentation/Legenda.xlsx
+++ b/Documentation/Legenda.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="43">
   <si>
     <t>Serializalble</t>
   </si>
@@ -132,6 +132,27 @@
   </si>
   <si>
     <t>IGameClient</t>
+  </si>
+  <si>
+    <t>IRekening</t>
+  </si>
+  <si>
+    <t>IKlant</t>
+  </si>
+  <si>
+    <t>Money</t>
+  </si>
+  <si>
+    <t>Balie</t>
+  </si>
+  <si>
+    <t>Bankiersessie</t>
+  </si>
+  <si>
+    <t>IBalie</t>
+  </si>
+  <si>
+    <t>IBankiersessie</t>
   </si>
 </sst>
 </file>
@@ -514,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,9 +546,12 @@
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -537,8 +561,17 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -547,8 +580,16 @@
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -557,8 +598,16 @@
         <v>5</v>
       </c>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -567,8 +616,16 @@
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -577,8 +634,16 @@
         <v>5</v>
       </c>
       <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -587,8 +652,15 @@
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -597,8 +669,16 @@
         <v>5</v>
       </c>
       <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -607,8 +687,16 @@
       <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -617,8 +705,11 @@
         <v>5</v>
       </c>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -627,8 +718,11 @@
       <c r="D10" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -637,8 +731,11 @@
         <v>5</v>
       </c>
       <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -647,8 +744,11 @@
       <c r="D12" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -657,8 +757,11 @@
         <v>5</v>
       </c>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -667,8 +770,11 @@
       <c r="D14" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -677,8 +783,11 @@
         <v>5</v>
       </c>
       <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -689,8 +798,11 @@
       <c r="D16" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -699,8 +811,11 @@
         <v>5</v>
       </c>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -711,8 +826,11 @@
       <c r="D18" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -721,8 +839,11 @@
         <v>5</v>
       </c>
       <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -733,8 +854,11 @@
       <c r="D20" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -743,8 +867,11 @@
         <v>5</v>
       </c>
       <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -755,8 +882,11 @@
       <c r="D22" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -765,8 +895,11 @@
         <v>5</v>
       </c>
       <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -775,8 +908,11 @@
       <c r="D24" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -785,8 +921,11 @@
         <v>5</v>
       </c>
       <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -795,8 +934,11 @@
       <c r="D26" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -805,8 +947,11 @@
         <v>5</v>
       </c>
       <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -815,8 +960,11 @@
       <c r="D28" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -825,8 +973,11 @@
         <v>5</v>
       </c>
       <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -835,8 +986,11 @@
       <c r="D30" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -845,8 +999,11 @@
         <v>5</v>
       </c>
       <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -855,8 +1012,11 @@
       <c r="D32" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -865,6 +1025,9 @@
         <v>5</v>
       </c>
       <c r="D33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>